<commit_message>
Created Coupled Model hpp files
decomposed top_model.hpp into three different coupled model hpp files that top_model now includes instead.
</commit_message>
<xml_diff>
--- a/MAJMAR_DEVS/top_model_connections.xlsx
+++ b/MAJMAR_DEVS/top_model_connections.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cadmium_v2\example\Assignment1_SYSC5104\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAJMAR_DEVS\MAJMAR_DEVS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{016235DE-EBC1-49F1-9862-42BB8CE35ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B23EBE-A7FD-494A-ACC8-24BAA3EBACE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7C0CCE08-7237-4040-8E61-443A5C20A60E}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{7C0CCE08-7237-4040-8E61-443A5C20A60E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -432,7 +432,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>